<commit_message>
feat: refactor core application structure to fix data persistence in XSLX file and improve UX.
</commit_message>
<xml_diff>
--- a/data/export_linkedin.xlsx
+++ b/data/export_linkedin.xlsx
@@ -2,34 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="11430" yWindow="7875" windowWidth="28035" windowHeight="22215" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -50,17 +43,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -423,21 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col width="15.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="102.140625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="34" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="38.42578125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="44.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="7" bestFit="1" customWidth="1" min="6" max="6"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -474,34 +456,604 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samer El Sokhon</t>
+          <t>Nicolas d'Avout d'Auerstaedt</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Senior IT Operations Engineer | Production Support &amp; Operational Lead | Critical Systems | 15+ Years Experience</t>
+          <t>Directeur de la Transformation Numérique</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RTE Réseau de Transport d'Electricité</t>
+          <t>Abeille Assurances</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fontenay-le-Fleury, Île-de-France, France</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/samer-el-sokhon/</t>
-        </is>
-      </c>
+          <t>Paris, Île-de-France, France</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/fabriceleyglene</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jérôme Vaucelle</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Responsable pilotage projets et PMO at MUTAVIE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MUTAVIE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/jvaucelle</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/laetitia-palatini-a3b49412b</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jacques CHEMAOUN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Directeur des Etudes Informatiques chez Abeille Assurances</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Abeille Assurances</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Greater Paris Metropolitan Region</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/jacques-chemaoun-43253790</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sandrine RACOUCHOT</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DSI chez Abeille Assurances - Ambassadrice du Club Décision DSI - Membre du conseil d'administration du CIGREF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Abeille Assurances</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bois-Colombes, Île-de-France, France</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/sandrine-racouchot-74aa0172</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cyril BAYON</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Directeur Expérience Utilisateurs</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Abeille Assurances</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Greater Paris Metropolitan Region</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/cyrilbayon</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Franck Bonnier</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Head of IT Transverse Department chez ArcelorMittal France</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ArcelorMittal</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/franck-bonnier-04033221</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Denis Dey</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Responsable de programme data</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ArcelorMittal</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Lille, Hauts-de-France, France</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/denis-dey-88167528</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Chankar Pourouchotamane</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Head of Data Office Group</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CMA CGM</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Greater Marseille Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/chankar-pourouchotamane-79a5687</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gabriel Fricout</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Head Of Data Intelligence Department chez ArcelorMittal France</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ArcelorMittal France</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Greater Metz Area</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/gabriel-fricout-35709913</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tharaud J.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Chief Data Officer / Head of Data Plateform Engineering</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PMU</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Brunoy, Île-de-France, France</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/jtharaud</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Matthieu Bonan</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Head of Data Office chez Groupe KILOUTOU</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Groupe KILOUTOU</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Lille, Hauts-de-France, France</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/matthieu-bonan-aa8263109</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Naceur Abderrahim</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Head of Data Management and Governance</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Servier</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Paris, Île-de-France, France</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/naceur-abderrahim-25b6b29</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Thierry Mocquillon</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Directeur Technologie et Système d’Information - Infrastructures, Technologies et Services</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Groupe Covéa</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>La Rochelle, Nouvelle-Aquitaine, France</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/thierry-mocquillon-39636236</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/alexandre-rouger-216899198</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Cyprien Falque</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Directeur général / CEO chez S3NS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>S3NS</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Greater Paris Metropolitan Region</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/cyprien-falque-05878131</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/olivier-esposito-861464155</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mickael DUPONT</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Actuaire / Data Scientist / Manager IT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Groupe Covéa</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Niort, Nouvelle-Aquitaine, France</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/mickael-dupont-61950810</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/david-brenet-ab26367b</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mehdy A.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Responsable Pôle Infrastructure chez APIVIA Courtage, filiale d'Apivia Macif Mutuelle - Aéma Groupe</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Apivia Courtage</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Poitiers, Nouvelle-Aquitaine, France</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/mehdy-a-4a865baa</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/cedric-porchier-43ba2a194</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>emmanuel Roquigny</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Responsable SIRH</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Inter Mutuelle Assistance</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Greater La Rochelle Area</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/emmanuel-roquigny-217521b6</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/fabien-leroy-70683070</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Olivier Louis MONNIER</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Group Chief Data &amp; AI Officer</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Paris, Île-de-France, France</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/olivier-louis-monnier</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/leverageondata</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Arnaud HAMEL</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Head of IT Architecture chez Rexel</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Rexel</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Greater Paris Metropolitan Region</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/arnaud-hamel-a1902665/</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add abstraction layer on browser to enable offline test
</commit_message>
<xml_diff>
--- a/data/export_linkedin.xlsx
+++ b/data/export_linkedin.xlsx
@@ -456,187 +456,187 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nicolas d'Avout d'Auerstaedt</t>
+          <t>Franck Bonnier</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Directeur de la Transformation Numérique</t>
+          <t>Head of IT Transverse Department chez ArcelorMittal France</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Abeille Assurances</t>
+          <t>ArcelorMittal</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Paris, Île-de-France, France</t>
+          <t>France</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+          <t>https://www.linkedin.com/in/franck-bonnier-04033221</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/fabriceleyglene</t>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jérôme Vaucelle</t>
+          <t>Denis Dey</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Responsable pilotage projets et PMO at MUTAVIE</t>
+          <t>Responsable de programme data</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MUTAVIE</t>
+          <t>ArcelorMittal</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Lille, Hauts-de-France, France</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/jvaucelle</t>
+          <t>https://www.linkedin.com/in/denis-dey-88167528</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/laetitia-palatini-a3b49412b</t>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jacques CHEMAOUN</t>
+          <t>Chankar Pourouchotamane</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Directeur des Etudes Informatiques chez Abeille Assurances</t>
+          <t>Head of Data Office Group</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Abeille Assurances</t>
+          <t>CMA CGM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Greater Paris Metropolitan Region</t>
+          <t>Greater Marseille Metropolitan Area</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/jacques-chemaoun-43253790</t>
+          <t>https://www.linkedin.com/in/chankar-pourouchotamane-79a5687</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sandrine RACOUCHOT</t>
+          <t>Gabriel Fricout</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DSI chez Abeille Assurances - Ambassadrice du Club Décision DSI - Membre du conseil d'administration du CIGREF</t>
+          <t>Head Of Data Intelligence Department chez ArcelorMittal France</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Abeille Assurances</t>
+          <t>ArcelorMittal France</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bois-Colombes, Île-de-France, France</t>
+          <t>Greater Metz Area</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/sandrine-racouchot-74aa0172</t>
+          <t>https://www.linkedin.com/in/gabriel-fricout-35709913</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cyril BAYON</t>
+          <t>Tharaud J.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Directeur Expérience Utilisateurs</t>
+          <t>Chief Data Officer / Head of Data Plateform Engineering</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Abeille Assurances</t>
+          <t>PMU</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Greater Paris Metropolitan Region</t>
+          <t>Brunoy, Île-de-France, France</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/cyrilbayon</t>
+          <t>https://www.linkedin.com/in/jtharaud</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Franck Bonnier</t>
+          <t>Matthieu Bonan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Head of IT Transverse Department chez ArcelorMittal France</t>
+          <t>Head of Data Office chez Groupe KILOUTOU</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ArcelorMittal</t>
+          <t>Groupe KILOUTOU</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Lille, Hauts-de-France, France</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/franck-bonnier-04033221</t>
+          <t>https://www.linkedin.com/in/matthieu-bonan-aa8263109</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -648,27 +648,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Denis Dey</t>
+          <t>Naceur Abderrahim</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Responsable de programme data</t>
+          <t>Head of Data Management and Governance</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ArcelorMittal</t>
+          <t>Servier</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Lille, Hauts-de-France, France</t>
+          <t>Paris, Île-de-France, France</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/denis-dey-88167528</t>
+          <t>https://www.linkedin.com/in/naceur-abderrahim-25b6b29</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,209 +680,205 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chankar Pourouchotamane</t>
+          <t>Thierry Mocquillon</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Head of Data Office Group</t>
+          <t>Directeur Technologie et Système d’Information - Infrastructures, Technologies et Services</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CMA CGM</t>
+          <t>Groupe Covéa</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Greater Marseille Metropolitan Area</t>
+          <t>La Rochelle, Nouvelle-Aquitaine, France</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/chankar-pourouchotamane-79a5687</t>
+          <t>https://www.linkedin.com/in/thierry-mocquillon-39636236</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+          <t>https://www.linkedin.com/in/alexandre-rouger-216899198</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Gabriel Fricout</t>
+          <t>Cyprien Falque</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Head Of Data Intelligence Department chez ArcelorMittal France</t>
+          <t>Directeur général / CEO chez S3NS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ArcelorMittal France</t>
+          <t>S3NS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Greater Metz Area</t>
+          <t>Greater Paris Metropolitan Region</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/gabriel-fricout-35709913</t>
+          <t>https://www.linkedin.com/in/cyprien-falque-05878131</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+          <t>https://www.linkedin.com/in/olivier-esposito-861464155</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tharaud J.</t>
+          <t>Mickael DUPONT</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Chief Data Officer / Head of Data Plateform Engineering</t>
+          <t>Actuaire / Data Scientist / Manager IT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PMU</t>
+          <t>Groupe Covéa</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Brunoy, Île-de-France, France</t>
+          <t>Niort, Nouvelle-Aquitaine, France</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/jtharaud</t>
+          <t>https://www.linkedin.com/in/mickael-dupont-61950810</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+          <t>https://www.linkedin.com/in/david-brenet-ab26367b</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Matthieu Bonan</t>
+          <t>Mehdy A.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Head of Data Office chez Groupe KILOUTOU</t>
+          <t>Responsable Pôle Infrastructure chez APIVIA Courtage, filiale d'Apivia Macif Mutuelle - Aéma Groupe</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Groupe KILOUTOU</t>
+          <t>Apivia Courtage</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Lille, Hauts-de-France, France</t>
+          <t>Poitiers, Nouvelle-Aquitaine, France</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/matthieu-bonan-aa8263109</t>
+          <t>https://www.linkedin.com/in/mehdy-a-4a865baa</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+          <t>https://www.linkedin.com/in/cedric-porchier-43ba2a194</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Naceur Abderrahim</t>
+          <t>emmanuel Roquigny</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Head of Data Management and Governance</t>
+          <t>Responsable SIRH</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Servier</t>
+          <t>Inter Mutuelle Assistance</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Paris, Île-de-France, France</t>
+          <t>Greater La Rochelle Area</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/naceur-abderrahim-25b6b29</t>
+          <t>https://www.linkedin.com/in/emmanuel-roquigny-217521b6</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/hamouda-makhloufi-934a7437</t>
+          <t>https://www.linkedin.com/in/fabien-leroy-70683070</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Thierry Mocquillon</t>
+          <t>Olivier Louis MONNIER</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Directeur Technologie et Système d’Information - Infrastructures, Technologies et Services</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Groupe Covéa</t>
-        </is>
-      </c>
+          <t>Group Chief Data &amp; AI Officer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>La Rochelle, Nouvelle-Aquitaine, France</t>
+          <t>Paris, Île-de-France, France</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/thierry-mocquillon-39636236</t>
+          <t>https://www.linkedin.com/in/olivier-louis-monnier</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/alexandre-rouger-216899198</t>
+          <t>https://www.linkedin.com/in/leverageondata</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Cyprien Falque</t>
+          <t>Arnaud HAMEL</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Directeur général / CEO chez S3NS</t>
+          <t>Head of IT Architecture chez Rexel</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>S3NS</t>
+          <t>Rexel</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -892,166 +888,170 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/cyprien-falque-05878131</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/olivier-esposito-861464155</t>
-        </is>
-      </c>
+          <t>https://www.linkedin.com/in/arnaud-hamel-a1902665/</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mickael DUPONT</t>
+          <t>Jean Dupont (Mock)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Actuaire / Data Scientist / Manager IT</t>
+          <t>Développeur Python Senior</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Groupe Covéa</t>
+          <t>Mock Corp</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Niort, Nouvelle-Aquitaine, France</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/mickael-dupont-61950810</t>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/david-brenet-ab26367b</t>
+          <t>https://www.linkedin.com/in/fabriceleyglene</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mehdy A.</t>
+          <t>Jean Dupont (Mock)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Responsable Pôle Infrastructure chez APIVIA Courtage, filiale d'Apivia Macif Mutuelle - Aéma Groupe</t>
+          <t>Développeur Python Senior</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Apivia Courtage</t>
+          <t>Mock Corp</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Poitiers, Nouvelle-Aquitaine, France</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/mehdy-a-4a865baa</t>
+          <t>https://www.linkedin.com/in/jvaucelle</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/cedric-porchier-43ba2a194</t>
+          <t>https://www.linkedin.com/in/laetitia-palatini-a3b49412b</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>emmanuel Roquigny</t>
+          <t>Jean Dupont (Mock)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Responsable SIRH</t>
+          <t>Développeur Python Senior</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Inter Mutuelle Assistance</t>
+          <t>Mock Corp</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Greater La Rochelle Area</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/emmanuel-roquigny-217521b6</t>
+          <t>https://www.linkedin.com/in/jacques-chemaoun-43253790</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/fabien-leroy-70683070</t>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Olivier Louis MONNIER</t>
+          <t>Jean Dupont (Mock)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Group Chief Data &amp; AI Officer</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>Développeur Python Senior</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Mock Corp</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Paris, Île-de-France, France</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/olivier-louis-monnier</t>
+          <t>https://www.linkedin.com/in/sandrine-racouchot-74aa0172</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/leverageondata</t>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Arnaud HAMEL</t>
+          <t>Jean Dupont (Mock)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Head of IT Architecture chez Rexel</t>
+          <t>Développeur Python Senior</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Rexel</t>
+          <t>Mock Corp</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Greater Paris Metropolitan Region</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/arnaud-hamel-a1902665/</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
+          <t>https://www.linkedin.com/in/cyrilbayon</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/nicolas-d-avout-d-auerstaedt-16201b53</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>